<commit_message>
abu Yousuf 4th push
</commit_message>
<xml_diff>
--- a/data/oussama-data.xlsx
+++ b/data/oussama-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/Desktop/FinalProjectTeam1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayran\OneDrive\Desktop\FinalProjectTeam1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29151670-9971-0943-A513-688C8D00024D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8BFCD7-631F-494C-A50D-F956802ECC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="oussama-data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>loginEmailForCustomer</t>
   </si>
@@ -53,13 +53,19 @@
   </si>
   <si>
     <t>UXdlcnR5JjEyMzQ1Njc</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>email1@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -71,6 +77,14 @@
       <sz val="18"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -117,15 +131,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,19 +458,19 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" customWidth="1"/>
-    <col min="2" max="2" width="62.83203125" customWidth="1"/>
+    <col min="1" max="1" width="47.36328125" customWidth="1"/>
+    <col min="2" max="2" width="62.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="36" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -461,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="35" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="39" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -477,7 +494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="34" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -485,7 +502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="35" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -493,7 +510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="39" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -501,7 +518,18 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:2" ht="39" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{A3DA162F-3264-48CF-A27D-8BE6995419B2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Abu Yousuf 6th Push
</commit_message>
<xml_diff>
--- a/data/oussama-data.xlsx
+++ b/data/oussama-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayran\OneDrive\Desktop\FinalProjectTeam1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8BFCD7-631F-494C-A50D-F956802ECC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E386296A-9025-4F93-9B79-2F60E5A16F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>loginEmailForCustomer</t>
   </si>
@@ -59,13 +59,56 @@
   </si>
   <si>
     <t>email1@gmail.com</t>
+  </si>
+  <si>
+    <t>ABU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fristName </t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>YOUSUF</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>US BANGLA CORP</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Admin1234</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>ABU YOUSUF</t>
+  </si>
+  <si>
+    <t>abuyousuf@yahoo.com</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Please feel free to contact me via email at emai786@gmail.com or by phone at 212-222-2222 to discuss further  details or
+provide any necessary information.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -85,6 +128,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF871094"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="4">
@@ -135,11 +183,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -458,10 +512,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -519,17 +573,83 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="39" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.5">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{A3DA162F-3264-48CF-A27D-8BE6995419B2}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{9BCBE943-7056-4528-B06C-1257326FF7EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Abu Yousuf 8th Push
</commit_message>
<xml_diff>
--- a/data/oussama-data.xlsx
+++ b/data/oussama-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayran\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayran\OneDrive\Desktop\FinalProjectTeam1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E757E73D-354C-4AEC-960B-DE1C9E7E1186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7765AB-FDA9-4970-BEC9-881B096BB9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>loginEmailForCustomer</t>
   </si>
@@ -183,6 +183,46 @@
   </si>
   <si>
     <t>abuyousuf@yahoo.com</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Please feel free to contact me via email at emai786@gmail.com or by phone at 212-222-2222 to discuss further  details or
+provide any necessary information.</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Delicate Blooms: A Review of the Flower Girl Bracelet</t>
+  </si>
+  <si>
+    <t>Overall, I highly recommend the Flower Girl Bracelet. Its delicate design, durability, and adjustable size make it an excellent choice for any young girl. Whether it's for a wedding, a special event, or just as a thoughtful gift, this bracelet is sure to bring joy and smiles to anyone who wears it.</t>
+  </si>
+  <si>
+    <t>reviewText</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>1000 Woodside Avenue</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>212-222-2222</t>
   </si>
 </sst>
 </file>
@@ -309,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -325,6 +365,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -644,10 +693,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -766,6 +815,62 @@
       </c>
       <c r="B14" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.5">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="14" customFormat="1">
+      <c r="A17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="13" customFormat="1">
+      <c r="A20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>